<commit_message>
Refactored some methods from the GUI class to the schedule class. Added a method to the GUI class which creates a schedule using a range of shortest shiftand longest shift to determine the optimal parameters
</commit_message>
<xml_diff>
--- a/ExcelFiles/Offices/3.CPCOM 140.xlsx
+++ b/ExcelFiles/Offices/3.CPCOM 140.xlsx
@@ -564,7 +564,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:F25"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1319,19 +1319,19 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="B26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26" s="12">
         <v>0</v>
@@ -1753,7 +1753,7 @@
       <c r="A41" s="21"/>
       <c r="B41" s="19">
         <f>SUM(B8:B40)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C41" s="19">
         <f>SUM(C1:C2)</f>
@@ -1784,7 +1784,7 @@
       <c r="A42" s="22"/>
       <c r="B42" s="19">
         <f>B41*5</f>
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>

</xml_diff>